<commit_message>
Adapt packageSuffix and overridePackage, and import classes.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoTypeReferenceKtTask.xlsx
+++ b/meta/program/BlancoTypeReferenceKtTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoTypeReferenceKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AE903B-BA31-014D-BAE7-F572E1F365AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7317EBD5-36C0-0545-80D2-B526122A85BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21280" yWindow="1400" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,7 @@
     <sheet name="config" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Submit有無">#REF!</definedName>
-    <definedName name="Validate実装パターン">#REF!</definedName>
-    <definedName name="チェック種別">#REF!</definedName>
-    <definedName name="デリミタ">#REF!</definedName>
-    <definedName name="デリミタ選択肢">#REF!</definedName>
-    <definedName name="型">#REF!</definedName>
     <definedName name="型リスト">config!$A$5:$A$12</definedName>
-    <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">config!$C$5:$C$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -397,6 +390,135 @@
   </si>
   <si>
     <t>BlancoTypeReferenceMap</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>searchTmpdir</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>voPackageSuffix</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>packageを探しにいくValueObject定義書を処理する際に指定されていたはずの packageSuffix を指定します。</t>
+    <rPh sb="8" eb="9">
+      <t xml:space="preserve">サガシニ </t>
+    </rPh>
+    <rPh sb="24" eb="27">
+      <t xml:space="preserve">テイギショヲ </t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t xml:space="preserve">ショリスル </t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t xml:space="preserve">サイニ </t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t xml:space="preserve">シテイサレテイタ </t>
+    </rPh>
+    <rPh sb="60" eb="62">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>voOverridePackage</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>packageを探しにいくValueObject定義書を処理する際に指定されていたはずの overridePackage を指定します。</t>
+    <rPh sb="8" eb="9">
+      <t xml:space="preserve">サガシニ </t>
+    </rPh>
+    <rPh sb="24" eb="27">
+      <t xml:space="preserve">テイギショヲ </t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t xml:space="preserve">ショリスル </t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t xml:space="preserve">サイニ </t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t xml:space="preserve">シテイサレテイタ </t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>import文作成のために検索するtmpディレクトリをカンマ区切りで指定します。指定ディレクトリ直下のvalueobjectディレクトリとrestgenratorディレクトリの下にxmlを探しにいきます。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>restPackageSuffix</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>restOverridePackage</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>restOverrideLocation</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>API定義書で指定されたパッケージ名の後ろに追加するパッケージ文字列を指定します。</t>
+    <rPh sb="3" eb="6">
+      <t xml:space="preserve">テイギショ </t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t xml:space="preserve">ウシロニ </t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t xml:space="preserve">ツイカ </t>
+    </rPh>
+    <rPh sb="31" eb="34">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>API定義書で指定されたパッケージ名を上書きします。</t>
+    <rPh sb="3" eb="6">
+      <t xml:space="preserve">テイギショ </t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t xml:space="preserve">ウワガキシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>API定義書で指定されたロケーション名を上書きします。</t>
+    <rPh sb="3" eb="6">
+      <t xml:space="preserve">テイギショ </t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t xml:space="preserve">ウワガキシマス。 </t>
+    </rPh>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -883,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -986,38 +1108,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1037,6 +1127,43 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1405,10 +1532,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:I24"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1454,10 +1581,10 @@
       <c r="F5"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="70"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="6" t="s">
         <v>52</v>
       </c>
@@ -1466,10 +1593,10 @@
       <c r="F6"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="70"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="6" t="s">
         <v>47</v>
       </c>
@@ -1480,10 +1607,10 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="70"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="6" t="s">
         <v>46</v>
       </c>
@@ -1494,10 +1621,10 @@
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="70"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
@@ -1528,38 +1655,38 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="75" t="s">
+      <c r="D12" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="76" t="s">
+      <c r="E12" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="65" t="s">
+      <c r="F12" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="74"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="1:9" ht="27" customHeight="1">
       <c r="A14" s="36">
@@ -1575,12 +1702,12 @@
         <v>13</v>
       </c>
       <c r="E14" s="40"/>
-      <c r="F14" s="71" t="s">
+      <c r="F14" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="73"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="61"/>
     </row>
     <row r="15" spans="1:9" ht="27" customHeight="1">
       <c r="A15" s="41">
@@ -1597,16 +1724,16 @@
       <c r="E15" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="61" t="s">
+      <c r="F15" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="63"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="70"/>
     </row>
     <row r="16" spans="1:9" ht="27" customHeight="1">
       <c r="A16" s="41">
-        <f t="shared" ref="A16:A28" si="0">A15+1</f>
+        <f t="shared" ref="A16:A33" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="42" t="s">
@@ -1619,12 +1746,12 @@
       <c r="E16" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="63"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="70"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="41">
@@ -1705,12 +1832,12 @@
       <c r="E20" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="67" t="s">
+      <c r="F20" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="69"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="76"/>
     </row>
     <row r="21" spans="1:10" ht="52" customHeight="1">
       <c r="A21" s="41">
@@ -1727,12 +1854,12 @@
       <c r="E21" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="58" t="s">
+      <c r="F21" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="59"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="60"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="67"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="41">
@@ -1749,12 +1876,12 @@
       <c r="E22" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="58" t="s">
+      <c r="F22" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="G22" s="59"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="60"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="67"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="41">
@@ -1771,12 +1898,12 @@
       <c r="E23" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="F23" s="58" t="s">
+      <c r="F23" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="60"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="67"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="41">
@@ -1793,12 +1920,12 @@
       <c r="E24" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="58" t="s">
+      <c r="F24" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="60"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="67"/>
     </row>
     <row r="25" spans="1:10" s="56" customFormat="1">
       <c r="A25" s="41">
@@ -1815,12 +1942,12 @@
       <c r="E25" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="F25" s="58" t="s">
+      <c r="F25" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="60"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="67"/>
       <c r="J25" s="55"/>
     </row>
     <row r="26" spans="1:10">
@@ -1836,12 +1963,12 @@
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="47"/>
-      <c r="F26" s="58" t="s">
+      <c r="F26" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="59"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="60"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="67"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="41">
@@ -1856,94 +1983,194 @@
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="47"/>
-      <c r="F27" s="58" t="s">
+      <c r="F27" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="60"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="67"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="41">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="60"/>
+      <c r="B28" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="44"/>
+      <c r="E28" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="70"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="17"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="22"/>
+      <c r="A29" s="77">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B29" s="78" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="54"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="55"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="17"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="22"/>
+      <c r="A30" s="77">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B30" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="54"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="55"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="17"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="34"/>
+      <c r="A31" s="77">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="D31" s="19"/>
       <c r="E31" s="20"/>
-      <c r="F31" s="21"/>
+      <c r="F31" s="79" t="s">
+        <v>73</v>
+      </c>
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
       <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="17"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="34"/>
+      <c r="A32" s="77">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="D32" s="19"/>
       <c r="E32" s="20"/>
-      <c r="F32" s="21"/>
+      <c r="F32" s="79" t="s">
+        <v>74</v>
+      </c>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
       <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="28"/>
+      <c r="A33" s="77">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="79" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="22"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="22"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="17"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="22"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="17"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="22"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="17"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="22"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="23"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D12:D13"/>
     <mergeCell ref="F28:I28"/>
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
@@ -1956,20 +2183,30 @@
     <mergeCell ref="F21:I21"/>
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="F23:I23"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F49" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F54" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D20 D26:D33 D22:D24" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D20 D22:D24 D26:D28 D31:D38" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C20 C26:C33 C22:C24" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C20 C22:C24 C26:C38" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>型リスト</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D25" xr:uid="{20C59D3E-A104-694F-8E50-28A1C51E7C99}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D25 D29:D30" xr:uid="{20C59D3E-A104-694F-8E50-28A1C51E7C99}">
       <formula1>必須</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>